<commit_message>
Upload part 1 report, part 3 experiment.
</commit_message>
<xml_diff>
--- a/submission/initial-analysis/javaFileSizes.xlsx
+++ b/submission/initial-analysis/javaFileSizes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/IdeaProjects/COM6523/individual-project/submission/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/home/IdeaProjects/COM6523/individual-project/submission/initial-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1391C163-A94C-D747-BA2B-68440FAEAD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EEF3B6-7AC8-7E44-9B3E-99C85E2CFBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="javaFileSizes" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,7 @@
     <definedName name="_xlchart.v1.1" hidden="1">javaFileSizes!$B$1</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">javaFileSizes!$B$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">javaFileSizes!$B$2:$B$168</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">javaFileSizes!$A$2:$A$168</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">javaFileSizes!$B$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">javaFileSizes!$B$2:$B$168</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">javaFileSizes!$A$2:$A$168</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">javaFileSizes!$B$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">javaFileSizes!$B$2:$B$168</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">javaFileSizes!$A$2:$A$168</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">javaFileSizes!$B$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">javaFileSizes!$B$2:$B$168</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">javaFileSizes!$B$2:$B$168</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">javaFileSizes!$A$2:$A$168</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">javaFileSizes!$B$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">javaFileSizes!$B$2:$B$168</definedName>
@@ -552,7 +543,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2341,158 +2332,163 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>11043</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1657</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>829491</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7303</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>828259</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>22087</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>649939</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>156713</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="3" name="Chart 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020EE285-9A6E-6747-8074-21FACBC3F4FA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2495826" y="200440"/>
-              <a:ext cx="7443303" cy="3200951"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6FC3354-4F33-6B4F-841B-34E24BF31967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="6205824" y="7303"/>
+          <a:ext cx="7313448" cy="7063854"/>
+          <a:chOff x="2432510" y="281056"/>
+          <a:chExt cx="7300748" cy="7267054"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+          <xdr:graphicFrame macro="">
+            <xdr:nvGraphicFramePr>
+              <xdr:cNvPr id="3" name="Chart 2">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020EE285-9A6E-6747-8074-21FACBC3F4FA}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvGraphicFramePr/>
+            </xdr:nvGraphicFramePr>
+            <xdr:xfrm>
+              <a:off x="2432510" y="281056"/>
+              <a:ext cx="7300748" cy="3637747"/>
+            </xdr:xfrm>
+            <a:graphic>
+              <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+                <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+              </a:graphicData>
+            </a:graphic>
+          </xdr:graphicFrame>
+        </mc:Choice>
+        <mc:Fallback>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="0" name=""/>
+              <xdr:cNvSpPr>
+                <a:spLocks noTextEdit="1"/>
+              </xdr:cNvSpPr>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="2432510" y="281056"/>
+                <a:ext cx="7300748" cy="3637747"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
               <a:solidFill>
-                <a:prstClr val="green"/>
+                <a:prstClr val="white"/>
               </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
+              <a:ln w="1">
+                <a:solidFill>
+                  <a:prstClr val="green"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>21535</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>176695</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="7" name="Chart 6">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1222E7FF-0424-7E48-AA9D-65D82266932E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2484784" y="3599622"/>
-              <a:ext cx="7454346" cy="5323508"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </mc:Fallback>
+      </mc:AlternateContent>
+      <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+        <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+          <xdr:graphicFrame macro="">
+            <xdr:nvGraphicFramePr>
+              <xdr:cNvPr id="7" name="Chart 6">
+                <a:extLst>
+                  <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                    <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1222E7FF-0424-7E48-AA9D-65D82266932E}"/>
+                  </a:ext>
+                </a:extLst>
+              </xdr:cNvPr>
+              <xdr:cNvGraphicFramePr/>
+            </xdr:nvGraphicFramePr>
+            <xdr:xfrm>
+              <a:off x="2433147" y="3911530"/>
+              <a:ext cx="7294179" cy="3636580"/>
+            </xdr:xfrm>
+            <a:graphic>
+              <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+                <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+              </a:graphicData>
+            </a:graphic>
+          </xdr:graphicFrame>
+        </mc:Choice>
+        <mc:Fallback>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="0" name=""/>
+              <xdr:cNvSpPr>
+                <a:spLocks noTextEdit="1"/>
+              </xdr:cNvSpPr>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="2433147" y="3911530"/>
+                <a:ext cx="7294179" cy="3636580"/>
+              </a:xfrm>
+              <a:prstGeom prst="rect">
+                <a:avLst/>
+              </a:prstGeom>
               <a:solidFill>
-                <a:prstClr val="green"/>
+                <a:prstClr val="white"/>
               </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t>This chart isn't available in your version of Excel.
+              <a:ln w="1">
+                <a:solidFill>
+                  <a:prstClr val="green"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100"/>
+                  <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+                </a:r>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </mc:Fallback>
+      </mc:AlternateContent>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2794,14 +2790,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="70.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>